<commit_message>
Updated jpg and theme of excel file
</commit_message>
<xml_diff>
--- a/assets/excel file/Catalog Database Example Sheet - OG.xlsx
+++ b/assets/excel file/Catalog Database Example Sheet - OG.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hao\Desktop\excel file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hao\Desktop\Hao Dong io\haodong191.github.io\assets\excel file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C4B80B-9E8C-4B6E-9C66-F6EAE39411BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72D5852-06B2-41C8-B1AA-0788BD81C88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{55169C12-04F5-4AC6-B71B-75EB8F464ABA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{55169C12-04F5-4AC6-B71B-75EB8F464ABA}"/>
   </bookViews>
   <sheets>
     <sheet name="Error Finder" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -805,12 +805,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -830,6 +824,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF064E41"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -937,9 +937,8 @@
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -962,28 +961,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1011,7 +1011,41 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.499984740745262"/>
+          <bgColor rgb="FF064E41"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF064E41"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -1052,58 +1086,6 @@
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1479,8 +1461,31 @@
         </top>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF064E41"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1493,18 +1498,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{302BE5E8-5980-4D57-A682-3690EF8737EC}" name="Table4" displayName="Table4" ref="A2:I102" totalsRowShown="0" headerRowDxfId="0" dataDxfId="18" tableBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{302BE5E8-5980-4D57-A682-3690EF8737EC}" name="Table4" displayName="Table4" ref="A2:I102" totalsRowShown="0" headerRowDxfId="1" dataDxfId="28" tableBorderDxfId="27">
   <autoFilter ref="A2:I102" xr:uid="{302BE5E8-5980-4D57-A682-3690EF8737EC}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{7EE139CF-391F-44C7-BE29-1AAE14FDB392}" name="Vendor Part Number" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{675A810B-ABA6-4E55-961F-962AF9A25072}" name="UPC" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{1EF08C87-CAB7-4FCB-A13D-BB182DD850FA}" name="Product Name" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{FE1DDF01-0C6E-464C-A5C4-BE39B9EDE444}" name="Unit(s)" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{B826574D-DB3D-4A55-AF9D-1521B85CFF28}" name="Count" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{696D9E6D-FF86-4B36-93D0-E0F5D17D0699}" name="Weight" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{AA77930A-2103-432B-8A60-44C137855939}" name="Class" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{88C9F4D7-4D86-42FF-9C61-6AE824EE00DB}" name="QTY" dataDxfId="20"/>
-    <tableColumn id="9" xr3:uid="{67F6A134-39B8-4E09-87AA-FE6643A2EA49}" name="In-House Part Number" dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{7EE139CF-391F-44C7-BE29-1AAE14FDB392}" name="Vendor Part Number" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{675A810B-ABA6-4E55-961F-962AF9A25072}" name="UPC" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{1EF08C87-CAB7-4FCB-A13D-BB182DD850FA}" name="Product Name" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{FE1DDF01-0C6E-464C-A5C4-BE39B9EDE444}" name="Unit(s)" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{B826574D-DB3D-4A55-AF9D-1521B85CFF28}" name="Count" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{696D9E6D-FF86-4B36-93D0-E0F5D17D0699}" name="Weight" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{AA77930A-2103-432B-8A60-44C137855939}" name="Class" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{88C9F4D7-4D86-42FF-9C61-6AE824EE00DB}" name="QTY" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{67F6A134-39B8-4E09-87AA-FE6643A2EA49}" name="In-House Part Number" dataDxfId="18">
       <calculatedColumnFormula>IF(G3="Office Supply", A3 &amp; "-OS", IF(G3="Food Product", A3 &amp; "-FP", "ERROR"))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1513,19 +1518,19 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F30C35A2-C738-412B-890A-ED85E6049062}" name="Table5" displayName="Table5" ref="A2:J96" totalsRowShown="0" headerRowDxfId="5" dataDxfId="6" tableBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F30C35A2-C738-412B-890A-ED85E6049062}" name="Table5" displayName="Table5" ref="A2:J96" totalsRowShown="0" headerRowDxfId="0" dataDxfId="17" tableBorderDxfId="16">
   <autoFilter ref="A2:J96" xr:uid="{F30C35A2-C738-412B-890A-ED85E6049062}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{A7A4EAF8-9053-4A15-BA82-0C09FF5FE296}" name="Vendor Part Number" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{0BDF5131-5CD7-4AD2-A8C4-231D238C4C6B}" name="Vendor Name" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{7BE1F134-0A7A-4A31-91A1-9074DF306AD1}" name="UPC" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{F83A1A27-399B-47E4-A89C-58C1931E32B0}" name="Product Name" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{D243E27D-EE14-412D-8265-D77F202EB22D}" name="Unit(s)" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{51565EED-A627-4DEB-BB15-87666DC2A9CC}" name="Count" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{951655C0-33CD-403A-8D6D-CAC7C0DC3949}" name="Weight" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{C164521F-9991-43EB-BBCA-BCD7A9E6559F}" name="Class" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{D6DCB013-FC71-4D63-AFA6-8793C37618BB}" name="QTY" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{4BF4D68D-289D-4773-8E97-C902898A8303}" name="In-House Part Number" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{A7A4EAF8-9053-4A15-BA82-0C09FF5FE296}" name="Vendor Part Number" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{0BDF5131-5CD7-4AD2-A8C4-231D238C4C6B}" name="Vendor Name" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{7BE1F134-0A7A-4A31-91A1-9074DF306AD1}" name="UPC" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{F83A1A27-399B-47E4-A89C-58C1931E32B0}" name="Product Name" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{D243E27D-EE14-412D-8265-D77F202EB22D}" name="Unit(s)" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{51565EED-A627-4DEB-BB15-87666DC2A9CC}" name="Count" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{951655C0-33CD-403A-8D6D-CAC7C0DC3949}" name="Weight" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{C164521F-9991-43EB-BBCA-BCD7A9E6559F}" name="Class" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{D6DCB013-FC71-4D63-AFA6-8793C37618BB}" name="QTY" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{4BF4D68D-289D-4773-8E97-C902898A8303}" name="In-House Part Number" dataDxfId="6">
       <calculatedColumnFormula>IF(H3="Office Supply", A3 &amp; "-OS", IF(H3="Food Product", A3 &amp; "-FP", "ERROR"))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1852,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A604505-050A-4197-9B8A-C8C318CBF549}">
   <dimension ref="A1:AA102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2:AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1886,117 +1891,117 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="23" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="17" t="s">
         <v>211</v>
       </c>
-      <c r="L1" s="6"/>
-      <c r="M1" s="24" t="s">
+      <c r="L1" s="5"/>
+      <c r="M1" s="18" t="s">
         <v>221</v>
       </c>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="24" t="s">
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
     </row>
     <row r="2" spans="1:27" ht="30" x14ac:dyDescent="0.4">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="21" t="s">
+      <c r="B2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="20" t="s">
         <v>213</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="20" t="s">
         <v>210</v>
       </c>
       <c r="J2" s="1"/>
-      <c r="K2" s="18">
+      <c r="K2" s="14">
         <f>COUNTA(M3:M1048576) + COUNTA(U3:U1048576)</f>
         <v>10</v>
       </c>
       <c r="L2" s="1"/>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="24" t="s">
         <v>201</v>
       </c>
-      <c r="N2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O2" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" s="17" t="s">
+      <c r="N2" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="17" t="s">
+      <c r="Q2" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="R2" s="17" t="s">
+      <c r="R2" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="S2" s="17" t="s">
+      <c r="S2" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="T2" s="7"/>
-      <c r="U2" s="17" t="s">
+      <c r="T2" s="6"/>
+      <c r="U2" s="24" t="s">
         <v>201</v>
       </c>
-      <c r="V2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="W2" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="X2" s="17" t="s">
+      <c r="V2" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="W2" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="X2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="Y2" s="17" t="s">
+      <c r="Y2" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="Z2" s="17" t="s">
+      <c r="Z2" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="AA2" s="17" t="s">
+      <c r="AA2" s="24" t="s">
         <v>198</v>
       </c>
     </row>
@@ -2032,49 +2037,49 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="20" t="str" cm="1">
+      <c r="M3" s="16" t="str" cm="1">
         <f t="array" ref="M3:S6">_xlfn._xlws.FILTER(A:G, I:I="ERROR", "No ERROR found")</f>
         <v>1234-033</v>
       </c>
-      <c r="N3" s="20">
+      <c r="N3" s="16">
         <v>72527273102</v>
       </c>
-      <c r="O3" s="20" t="str">
+      <c r="O3" s="16" t="str">
         <v>Pig Feed</v>
       </c>
-      <c r="P3" s="20">
+      <c r="P3" s="16">
         <v>18</v>
       </c>
-      <c r="Q3" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="R3" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="S3" s="20" t="str">
+      <c r="Q3" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="R3" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="S3" s="16" t="str">
         <v>Farm Supply</v>
       </c>
       <c r="T3" s="1"/>
-      <c r="U3" s="20" t="str" cm="1">
+      <c r="U3" s="16" t="str" cm="1">
         <f t="array" ref="U3:AA8">_xlfn._xlws.FILTER(A2:G102, B2:B102="", "No blank cells found")</f>
         <v>1234-010</v>
       </c>
-      <c r="V3" s="20">
-        <v>0</v>
-      </c>
-      <c r="W3" s="20" t="str">
+      <c r="V3" s="16">
+        <v>0</v>
+      </c>
+      <c r="W3" s="16" t="str">
         <v>Filing Cabinet</v>
       </c>
-      <c r="X3" s="20">
+      <c r="X3" s="16">
         <v>20</v>
       </c>
-      <c r="Y3" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="20" t="str">
+      <c r="Y3" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="16" t="str">
         <v>Office Supply</v>
       </c>
     </row>
@@ -2110,47 +2115,47 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="20" t="str">
+      <c r="M4" s="16" t="str">
         <v>1234-042</v>
       </c>
-      <c r="N4" s="20">
+      <c r="N4" s="16">
         <v>72527273111</v>
       </c>
-      <c r="O4" s="20" t="str">
+      <c r="O4" s="16" t="str">
         <v>Hot Wheel</v>
       </c>
-      <c r="P4" s="20">
+      <c r="P4" s="16">
         <v>36</v>
       </c>
-      <c r="Q4" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="R4" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="S4" s="20" t="str">
+      <c r="Q4" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="R4" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="S4" s="16" t="str">
         <v>Toy</v>
       </c>
       <c r="T4" s="1"/>
-      <c r="U4" s="20" t="str">
+      <c r="U4" s="16" t="str">
         <v>1234-024</v>
       </c>
-      <c r="V4" s="20">
-        <v>0</v>
-      </c>
-      <c r="W4" s="20" t="str">
+      <c r="V4" s="16">
+        <v>0</v>
+      </c>
+      <c r="W4" s="16" t="str">
         <v>Desk Mat</v>
       </c>
-      <c r="X4" s="20">
+      <c r="X4" s="16">
         <v>48</v>
       </c>
-      <c r="Y4" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="20" t="str">
+      <c r="Y4" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="16" t="str">
         <v>Office Supply</v>
       </c>
     </row>
@@ -2186,47 +2191,47 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="20" t="str">
+      <c r="M5" s="16" t="str">
         <v>1234-054</v>
       </c>
-      <c r="N5" s="20">
+      <c r="N5" s="16">
         <v>72527273123</v>
       </c>
-      <c r="O5" s="20" t="str">
+      <c r="O5" s="16" t="str">
         <v>Nikon T5i</v>
       </c>
-      <c r="P5" s="20">
+      <c r="P5" s="16">
         <v>12</v>
       </c>
-      <c r="Q5" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="R5" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="S5" s="20" t="str">
+      <c r="Q5" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="R5" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="S5" s="16" t="str">
         <v>Camera</v>
       </c>
       <c r="T5" s="1"/>
-      <c r="U5" s="20" t="str">
+      <c r="U5" s="16" t="str">
         <v>1234-035</v>
       </c>
-      <c r="V5" s="20">
-        <v>0</v>
-      </c>
-      <c r="W5" s="20" t="str">
+      <c r="V5" s="16">
+        <v>0</v>
+      </c>
+      <c r="W5" s="16" t="str">
         <v>Mechanical Keyboard</v>
       </c>
-      <c r="X5" s="20">
+      <c r="X5" s="16">
         <v>22</v>
       </c>
-      <c r="Y5" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA5" s="20" t="str">
+      <c r="Y5" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="16" t="str">
         <v>Office Supply</v>
       </c>
     </row>
@@ -2262,47 +2267,47 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="20" t="str">
+      <c r="M6" s="16" t="str">
         <v>1234-069</v>
       </c>
-      <c r="N6" s="20">
+      <c r="N6" s="16">
         <v>72527273138</v>
       </c>
-      <c r="O6" s="20" t="str">
+      <c r="O6" s="16" t="str">
         <v>Dawn Dish Soap</v>
       </c>
-      <c r="P6" s="20">
+      <c r="P6" s="16">
         <v>42</v>
       </c>
-      <c r="Q6" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="R6" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="S6" s="20" t="str">
+      <c r="Q6" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="R6" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="S6" s="16" t="str">
         <v>Cleaning Supply</v>
       </c>
       <c r="T6" s="1"/>
-      <c r="U6" s="20" t="str">
+      <c r="U6" s="16" t="str">
         <v>1234-051</v>
       </c>
-      <c r="V6" s="20">
-        <v>0</v>
-      </c>
-      <c r="W6" s="20" t="str">
+      <c r="V6" s="16">
+        <v>0</v>
+      </c>
+      <c r="W6" s="16" t="str">
         <v>Binder Folder</v>
       </c>
-      <c r="X6" s="20">
+      <c r="X6" s="16">
         <v>6</v>
       </c>
-      <c r="Y6" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="20" t="str">
+      <c r="Y6" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="16" t="str">
         <v>Office Supply</v>
       </c>
     </row>
@@ -2346,25 +2351,25 @@
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
-      <c r="U7" s="20" t="str">
+      <c r="U7" s="16" t="str">
         <v>1234-065</v>
       </c>
-      <c r="V7" s="20">
-        <v>0</v>
-      </c>
-      <c r="W7" s="20" t="str">
+      <c r="V7" s="16">
+        <v>0</v>
+      </c>
+      <c r="W7" s="16" t="str">
         <v>All-Purpose Flour</v>
       </c>
-      <c r="X7" s="20">
+      <c r="X7" s="16">
         <v>34</v>
       </c>
-      <c r="Y7" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA7" s="20" t="str">
+      <c r="Y7" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="16" t="str">
         <v>Food Product</v>
       </c>
     </row>
@@ -2408,25 +2413,25 @@
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
-      <c r="U8" s="20" t="str">
+      <c r="U8" s="16" t="str">
         <v>1234-082</v>
       </c>
-      <c r="V8" s="20">
-        <v>0</v>
-      </c>
-      <c r="W8" s="20" t="str">
+      <c r="V8" s="16">
+        <v>0</v>
+      </c>
+      <c r="W8" s="16" t="str">
         <v>Yogurt Cups</v>
       </c>
-      <c r="X8" s="20">
+      <c r="X8" s="16">
         <v>20</v>
       </c>
-      <c r="Y8" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA8" s="20" t="str">
+      <c r="Y8" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="16" t="str">
         <v>Food Product</v>
       </c>
     </row>
@@ -6945,8 +6950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5591908-A046-4C55-BA05-40C9131C2C97}">
   <dimension ref="A1:W96"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6976,96 +6981,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="L1" s="4" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="L1" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="N1" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="21"/>
+      <c r="W1" s="21"/>
     </row>
     <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="21" t="s">
+      <c r="C2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="20" t="s">
         <v>213</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="20" t="s">
         <v>210</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="2" t="s">
+      <c r="L2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="23" t="s">
         <v>216</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R2" s="2" t="s">
+      <c r="P2" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S2" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="T2" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="U2" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="V2" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="W2" s="23" t="s">
         <v>210</v>
       </c>
     </row>
@@ -7101,42 +7106,42 @@
         <f>IF(H3="Office Supply", A3 &amp; "-OS", IF(H3="Food Product", A3 &amp; "-FP", "ERROR"))</f>
         <v>1234-001-OS</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="L3" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="M3" s="14"/>
-      <c r="N3" s="5" t="str" cm="1">
+      <c r="M3" s="13"/>
+      <c r="N3" s="4" t="str" cm="1">
         <f t="array" ref="N3:W6">_xlfn._xlws.SORT(
     _xlfn._xlws.FILTER(A:J, ISNUMBER(SEARCH(L3, D:D)), "No match"),
     9, -1
 )</f>
         <v>1234-077</v>
       </c>
-      <c r="O3" s="5" t="str">
+      <c r="O3" s="4" t="str">
         <v>Aecme</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3" s="4">
         <v>72527273074</v>
       </c>
-      <c r="Q3" s="5" t="str">
+      <c r="Q3" s="4" t="str">
         <v>Gala Apples</v>
       </c>
-      <c r="R3" s="5">
+      <c r="R3" s="4">
         <v>10</v>
       </c>
-      <c r="S3" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T3" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="U3" s="5" t="str">
+      <c r="S3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T3" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="U3" s="4" t="str">
         <v>Food Product</v>
       </c>
-      <c r="V3" s="5">
+      <c r="V3" s="4">
         <v>30</v>
       </c>
-      <c r="W3" s="5" t="str">
+      <c r="W3" s="4" t="str">
         <v>1234-077-FP</v>
       </c>
     </row>
@@ -7172,36 +7177,36 @@
         <f t="shared" ref="J4:J24" si="0">IF(H4="Office Supply", A4 &amp; "-OS", IF(H4="Food Product", A4 &amp; "-FP", "ERROR"))</f>
         <v>1234-002-FP</v>
       </c>
-      <c r="L4" s="13"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="5" t="str">
+      <c r="L4" s="12"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="4" t="str">
         <v>1234-029</v>
       </c>
-      <c r="O4" s="5" t="str">
+      <c r="O4" s="4" t="str">
         <v>Top Teir Distribution</v>
       </c>
-      <c r="P4" s="5">
+      <c r="P4" s="4">
         <v>72527273074</v>
       </c>
-      <c r="Q4" s="5" t="str">
+      <c r="Q4" s="4" t="str">
         <v>Gala Apples</v>
       </c>
-      <c r="R4" s="5">
+      <c r="R4" s="4">
         <v>10</v>
       </c>
-      <c r="S4" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T4" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="U4" s="5" t="str">
+      <c r="S4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="U4" s="4" t="str">
         <v>Food Product</v>
       </c>
-      <c r="V4" s="5">
+      <c r="V4" s="4">
         <v>14</v>
       </c>
-      <c r="W4" s="5" t="str">
+      <c r="W4" s="4" t="str">
         <v>1234-029-FP</v>
       </c>
     </row>
@@ -7237,36 +7242,36 @@
         <f t="shared" si="0"/>
         <v>1234-003-OS</v>
       </c>
-      <c r="L5" s="12"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="5" t="str">
+      <c r="L5" s="11"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="4" t="str">
         <v>1234-005</v>
       </c>
-      <c r="O5" s="5" t="str">
+      <c r="O5" s="4" t="str">
         <v>Northeast Distribution</v>
       </c>
-      <c r="P5" s="5">
+      <c r="P5" s="4">
         <v>72527273074</v>
       </c>
-      <c r="Q5" s="5" t="str">
+      <c r="Q5" s="4" t="str">
         <v>Gala Apples</v>
       </c>
-      <c r="R5" s="5">
+      <c r="R5" s="4">
         <v>10</v>
       </c>
-      <c r="S5" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T5" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="U5" s="5" t="str">
+      <c r="S5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T5" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="U5" s="4" t="str">
         <v>Food Product</v>
       </c>
-      <c r="V5" s="5">
-        <v>0</v>
-      </c>
-      <c r="W5" s="5" t="str">
+      <c r="V5" s="4">
+        <v>0</v>
+      </c>
+      <c r="W5" s="4" t="str">
         <v>1234-005-FP</v>
       </c>
     </row>
@@ -7302,38 +7307,38 @@
         <f t="shared" si="0"/>
         <v>1234-004-OS</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="M6" s="3"/>
-      <c r="N6" s="5" t="str">
+      <c r="M6" s="2"/>
+      <c r="N6" s="4" t="str">
         <v>1234-053</v>
       </c>
-      <c r="O6" s="5" t="str">
+      <c r="O6" s="4" t="str">
         <v xml:space="preserve">You-Line </v>
       </c>
-      <c r="P6" s="5">
+      <c r="P6" s="4">
         <v>72527273074</v>
       </c>
-      <c r="Q6" s="5" t="str">
+      <c r="Q6" s="4" t="str">
         <v>Gala Apples</v>
       </c>
-      <c r="R6" s="5">
+      <c r="R6" s="4">
         <v>10</v>
       </c>
-      <c r="S6" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T6" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="U6" s="5" t="str">
+      <c r="S6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T6" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="U6" s="4" t="str">
         <v>Food Product</v>
       </c>
-      <c r="V6" s="5">
-        <v>0</v>
-      </c>
-      <c r="W6" s="5" t="str">
+      <c r="V6" s="4">
+        <v>0</v>
+      </c>
+      <c r="W6" s="4" t="str">
         <v>1234-053-FP</v>
       </c>
     </row>
@@ -7369,10 +7374,10 @@
         <f t="shared" si="0"/>
         <v>1234-005-FP</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="L7" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="M7" s="3"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -7406,10 +7411,10 @@
         <f t="shared" si="0"/>
         <v>1234-006-FP</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="L8" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="M8" s="3"/>
+      <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -7443,10 +7448,10 @@
         <f t="shared" si="0"/>
         <v>1234-007-OS</v>
       </c>
-      <c r="L9" s="10" t="s">
+      <c r="L9" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="M9" s="3"/>
+      <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -7480,10 +7485,10 @@
         <f t="shared" si="0"/>
         <v>1234-009-FP</v>
       </c>
-      <c r="L10" s="10" t="s">
+      <c r="L10" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="M10" s="3"/>
+      <c r="M10" s="2"/>
     </row>
     <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -7517,7 +7522,7 @@
         <f t="shared" si="0"/>
         <v>1234-011-FP</v>
       </c>
-      <c r="L11" s="10" t="s">
+      <c r="L11" s="9" t="s">
         <v>109</v>
       </c>
     </row>
@@ -7553,7 +7558,7 @@
         <f t="shared" si="0"/>
         <v>1234-012-OS</v>
       </c>
-      <c r="L12" s="10" t="s">
+      <c r="L12" s="9" t="s">
         <v>105</v>
       </c>
     </row>
@@ -7589,7 +7594,7 @@
         <f t="shared" si="0"/>
         <v>1234-013-OS</v>
       </c>
-      <c r="L13" s="10" t="s">
+      <c r="L13" s="9" t="s">
         <v>112</v>
       </c>
     </row>
@@ -7625,7 +7630,7 @@
         <f t="shared" si="0"/>
         <v>1234-014-FP</v>
       </c>
-      <c r="L14" s="10" t="s">
+      <c r="L14" s="9" t="s">
         <v>125</v>
       </c>
     </row>
@@ -7661,7 +7666,7 @@
         <f t="shared" si="0"/>
         <v>1234-015-FP</v>
       </c>
-      <c r="L15" s="9"/>
+      <c r="L15" s="8"/>
     </row>
     <row r="16" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -7695,7 +7700,7 @@
         <f t="shared" si="0"/>
         <v>1234-016-OS</v>
       </c>
-      <c r="L16" s="9"/>
+      <c r="L16" s="8"/>
     </row>
     <row r="17" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
@@ -7729,7 +7734,7 @@
         <f t="shared" si="0"/>
         <v>1234-017-FP</v>
       </c>
-      <c r="L17" s="9"/>
+      <c r="L17" s="8"/>
     </row>
     <row r="18" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
@@ -7763,7 +7768,7 @@
         <f t="shared" si="0"/>
         <v>1234-018-OS</v>
       </c>
-      <c r="L18" s="9"/>
+      <c r="L18" s="8"/>
     </row>
     <row r="19" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
@@ -7797,7 +7802,7 @@
         <f t="shared" si="0"/>
         <v>1234-019-OS</v>
       </c>
-      <c r="L19" s="9"/>
+      <c r="L19" s="8"/>
     </row>
     <row r="20" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
@@ -7831,7 +7836,7 @@
         <f t="shared" si="0"/>
         <v>1234-020-FP</v>
       </c>
-      <c r="L20" s="9"/>
+      <c r="L20" s="8"/>
     </row>
     <row r="21" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
@@ -7865,7 +7870,7 @@
         <f t="shared" si="0"/>
         <v>1234-021-OS</v>
       </c>
-      <c r="L21" s="9"/>
+      <c r="L21" s="8"/>
     </row>
     <row r="22" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
@@ -7899,7 +7904,7 @@
         <f t="shared" si="0"/>
         <v>1234-022-FP</v>
       </c>
-      <c r="L22" s="9"/>
+      <c r="L22" s="8"/>
     </row>
     <row r="23" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
@@ -7933,7 +7938,7 @@
         <f t="shared" si="0"/>
         <v>1234-023-FP</v>
       </c>
-      <c r="L23" s="9"/>
+      <c r="L23" s="8"/>
     </row>
     <row r="24" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
@@ -7967,7 +7972,7 @@
         <f t="shared" si="0"/>
         <v>1234-024-OS</v>
       </c>
-      <c r="L24" s="9"/>
+      <c r="L24" s="8"/>
     </row>
     <row r="25" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
@@ -8001,7 +8006,7 @@
         <f>IF(H25="Office Supply", A25 &amp; "-OS", IF(H25="Food Product", A25 &amp; "-FP", "ERROR"))</f>
         <v>1234-025-OS</v>
       </c>
-      <c r="L25" s="9"/>
+      <c r="L25" s="8"/>
     </row>
     <row r="26" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
@@ -8035,7 +8040,7 @@
         <f t="shared" ref="J26:J48" si="1">IF(H26="Office Supply", A26 &amp; "-OS", IF(H26="Food Product", A26 &amp; "-FP", "ERROR"))</f>
         <v>1234-026-FP</v>
       </c>
-      <c r="L26" s="9"/>
+      <c r="L26" s="8"/>
     </row>
     <row r="27" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
@@ -8069,7 +8074,7 @@
         <f t="shared" si="1"/>
         <v>1234-027-OS</v>
       </c>
-      <c r="L27" s="9"/>
+      <c r="L27" s="8"/>
     </row>
     <row r="28" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
@@ -8103,7 +8108,7 @@
         <f t="shared" si="1"/>
         <v>1234-028-OS</v>
       </c>
-      <c r="L28" s="9"/>
+      <c r="L28" s="8"/>
     </row>
     <row r="29" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
@@ -10355,16 +10360,16 @@
     <mergeCell ref="A1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="N3:W6">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>AND($V3&gt;=11, $V3&lt;=19)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$V3&lt;1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>$V3&gt;20</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>AND($V3&gt;=2, $V3&lt;=10)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>